<commit_message>
Completed All USB parts
</commit_message>
<xml_diff>
--- a/Eagle Tools/lbr/PARTS.xlsx
+++ b/Eagle Tools/lbr/PARTS.xlsx
@@ -6,12 +6,13 @@
   </bookViews>
   <sheets>
     <sheet name="Transistor" sheetId="1" r:id="rId4"/>
+    <sheet name="Connector" sheetId="2" r:id="rId5"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="99">
   <si>
     <t>BJT</t>
   </si>
@@ -209,6 +210,105 @@
   </si>
   <si>
     <t>SOD-323</t>
+  </si>
+  <si>
+    <t>USB</t>
+  </si>
+  <si>
+    <t>47346-0001</t>
+  </si>
+  <si>
+    <t>10033526-N3212MLF</t>
+  </si>
+  <si>
+    <t>48037-2200</t>
+  </si>
+  <si>
+    <t>UE27-AC54-100</t>
+  </si>
+  <si>
+    <t>UE27-AE54-100</t>
+  </si>
+  <si>
+    <t>87583-2010BLF</t>
+  </si>
+  <si>
+    <t>61729-0010BLF</t>
+  </si>
+  <si>
+    <t>MOLEX</t>
+  </si>
+  <si>
+    <t>Amphenol FCI</t>
+  </si>
+  <si>
+    <t>Amphenol</t>
+  </si>
+  <si>
+    <t>USB Type</t>
+  </si>
+  <si>
+    <t>Micro USB Type B Receptacle</t>
+  </si>
+  <si>
+    <t>Mini USB Type B Receptacle</t>
+  </si>
+  <si>
+    <t>USB Type A Plug</t>
+  </si>
+  <si>
+    <t>USB Type A Receptacle</t>
+  </si>
+  <si>
+    <t>USB Type B Receptacle</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Standard</t>
+  </si>
+  <si>
+    <t>USB 2.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Current Rating </t>
+  </si>
+  <si>
+    <t>1.8 A </t>
+  </si>
+  <si>
+    <t>1.5A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Voltage Rating </t>
+  </si>
+  <si>
+    <t>30 VAC</t>
+  </si>
+  <si>
+    <t>150 VAC</t>
+  </si>
+  <si>
+    <t>- 20 C to + 85 C</t>
+  </si>
+  <si>
+    <t>Through Hole</t>
+  </si>
+  <si>
+    <t>Mounting Angle</t>
+  </si>
+  <si>
+    <t>Right</t>
+  </si>
+  <si>
+    <t>Vertical</t>
   </si>
 </sst>
 </file>
@@ -301,7 +401,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -325,6 +425,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1809,4 +1915,292 @@
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:H10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.8333" defaultRowHeight="25.4" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1" width="61" style="8" customWidth="1"/>
+    <col min="2" max="2" width="38.8516" style="8" customWidth="1"/>
+    <col min="3" max="3" width="38.875" style="8" customWidth="1"/>
+    <col min="4" max="4" width="38.875" style="8" customWidth="1"/>
+    <col min="5" max="5" width="38.875" style="8" customWidth="1"/>
+    <col min="6" max="6" width="38.875" style="8" customWidth="1"/>
+    <col min="7" max="7" width="38.875" style="8" customWidth="1"/>
+    <col min="8" max="8" width="38.875" style="8" customWidth="1"/>
+    <col min="9" max="256" width="10.8516" style="8" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="23" customHeight="1">
+      <c r="A1" t="s" s="2">
+        <v>66</v>
+      </c>
+      <c r="B1" t="s" s="2">
+        <v>67</v>
+      </c>
+      <c r="C1" t="s" s="2">
+        <v>68</v>
+      </c>
+      <c r="D1" t="s" s="2">
+        <v>69</v>
+      </c>
+      <c r="E1" t="s" s="2">
+        <v>70</v>
+      </c>
+      <c r="F1" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="G1" t="s" s="2">
+        <v>72</v>
+      </c>
+      <c r="H1" t="s" s="2">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" ht="26" customHeight="1">
+      <c r="A2" t="s" s="3">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s" s="4">
+        <v>74</v>
+      </c>
+      <c r="C2" t="s" s="9">
+        <v>75</v>
+      </c>
+      <c r="D2" t="s" s="4">
+        <v>74</v>
+      </c>
+      <c r="E2" t="s" s="9">
+        <v>76</v>
+      </c>
+      <c r="F2" t="s" s="9">
+        <v>76</v>
+      </c>
+      <c r="G2" t="s" s="9">
+        <v>75</v>
+      </c>
+      <c r="H2" t="s" s="9">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" ht="26" customHeight="1">
+      <c r="A3" t="s" s="5">
+        <v>77</v>
+      </c>
+      <c r="B3" t="s" s="6">
+        <v>78</v>
+      </c>
+      <c r="C3" t="s" s="6">
+        <v>79</v>
+      </c>
+      <c r="D3" t="s" s="6">
+        <v>80</v>
+      </c>
+      <c r="E3" t="s" s="6">
+        <v>81</v>
+      </c>
+      <c r="F3" t="s" s="6">
+        <v>81</v>
+      </c>
+      <c r="G3" t="s" s="6">
+        <v>81</v>
+      </c>
+      <c r="H3" t="s" s="6">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" ht="26" customHeight="1">
+      <c r="A4" t="s" s="3">
+        <v>83</v>
+      </c>
+      <c r="B4" t="s" s="4">
+        <v>84</v>
+      </c>
+      <c r="C4" t="s" s="4">
+        <v>84</v>
+      </c>
+      <c r="D4" t="s" s="4">
+        <v>85</v>
+      </c>
+      <c r="E4" t="s" s="4">
+        <v>84</v>
+      </c>
+      <c r="F4" t="s" s="4">
+        <v>84</v>
+      </c>
+      <c r="G4" t="s" s="4">
+        <v>84</v>
+      </c>
+      <c r="H4" t="s" s="4">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" ht="26" customHeight="1">
+      <c r="A5" t="s" s="5">
+        <v>86</v>
+      </c>
+      <c r="B5" t="s" s="6">
+        <v>87</v>
+      </c>
+      <c r="C5" t="s" s="6">
+        <v>87</v>
+      </c>
+      <c r="D5" t="s" s="6">
+        <v>66</v>
+      </c>
+      <c r="E5" t="s" s="6">
+        <v>87</v>
+      </c>
+      <c r="F5" t="s" s="6">
+        <v>87</v>
+      </c>
+      <c r="G5" t="s" s="6">
+        <v>87</v>
+      </c>
+      <c r="H5" t="s" s="6">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" ht="26" customHeight="1">
+      <c r="A6" t="s" s="3">
+        <v>88</v>
+      </c>
+      <c r="B6" t="s" s="4">
+        <v>89</v>
+      </c>
+      <c r="C6" t="s" s="4">
+        <v>62</v>
+      </c>
+      <c r="D6" t="s" s="4">
+        <v>90</v>
+      </c>
+      <c r="E6" t="s" s="4">
+        <v>62</v>
+      </c>
+      <c r="F6" t="s" s="4">
+        <v>62</v>
+      </c>
+      <c r="G6" t="s" s="4">
+        <v>62</v>
+      </c>
+      <c r="H6" t="s" s="4">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" ht="26" customHeight="1">
+      <c r="A7" t="s" s="5">
+        <v>91</v>
+      </c>
+      <c r="B7" t="s" s="6">
+        <v>92</v>
+      </c>
+      <c r="C7" t="s" s="6">
+        <v>62</v>
+      </c>
+      <c r="D7" t="s" s="6">
+        <v>93</v>
+      </c>
+      <c r="E7" t="s" s="6">
+        <v>62</v>
+      </c>
+      <c r="F7" t="s" s="6">
+        <v>62</v>
+      </c>
+      <c r="G7" t="s" s="6">
+        <v>62</v>
+      </c>
+      <c r="H7" t="s" s="6">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" ht="26" customHeight="1">
+      <c r="A8" t="s" s="3">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s" s="4">
+        <v>94</v>
+      </c>
+      <c r="C8" t="s" s="4">
+        <v>62</v>
+      </c>
+      <c r="D8" t="s" s="4">
+        <v>94</v>
+      </c>
+      <c r="E8" t="s" s="4">
+        <v>62</v>
+      </c>
+      <c r="F8" t="s" s="4">
+        <v>62</v>
+      </c>
+      <c r="G8" t="s" s="4">
+        <v>62</v>
+      </c>
+      <c r="H8" t="s" s="4">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" ht="26" customHeight="1">
+      <c r="A9" t="s" s="5">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="D9" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="E9" t="s" s="6">
+        <v>95</v>
+      </c>
+      <c r="F9" t="s" s="6">
+        <v>95</v>
+      </c>
+      <c r="G9" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="H9" t="s" s="6">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="10" ht="26" customHeight="1">
+      <c r="A10" t="s" s="3">
+        <v>96</v>
+      </c>
+      <c r="B10" t="s" s="4">
+        <v>97</v>
+      </c>
+      <c r="C10" t="s" s="4">
+        <v>97</v>
+      </c>
+      <c r="D10" t="s" s="4">
+        <v>97</v>
+      </c>
+      <c r="E10" t="s" s="4">
+        <v>97</v>
+      </c>
+      <c r="F10" t="s" s="4">
+        <v>98</v>
+      </c>
+      <c r="G10" t="s" s="4">
+        <v>97</v>
+      </c>
+      <c r="H10" t="s" s="4">
+        <v>97</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Designed Realtek Ameba DEV01 shield
</commit_message>
<xml_diff>
--- a/Eagle Tools/lbr/PARTS.xlsx
+++ b/Eagle Tools/lbr/PARTS.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="116">
   <si>
     <t>BJT</t>
   </si>
@@ -20,7 +20,7 @@
     <t>BC850C,215</t>
   </si>
   <si>
-    <t>Column1</t>
+    <t>EMPTY</t>
   </si>
   <si>
     <t>Manufacturer</t>
@@ -309,6 +309,57 @@
   </si>
   <si>
     <t>Vertical</t>
+  </si>
+  <si>
+    <t>RJ45-ETHERNET</t>
+  </si>
+  <si>
+    <t>SI-68002</t>
+  </si>
+  <si>
+    <t>Magjack</t>
+  </si>
+  <si>
+    <t>Tyco</t>
+  </si>
+  <si>
+    <t>RJ45 Type</t>
+  </si>
+  <si>
+    <t>DEBUG CONNECTOR</t>
+  </si>
+  <si>
+    <t>TC2030-CTX</t>
+  </si>
+  <si>
+    <t>Tag Connect</t>
+  </si>
+  <si>
+    <t>Connector Type</t>
+  </si>
+  <si>
+    <t>6-PIN SWD</t>
+  </si>
+  <si>
+    <t>10-PIN SWD</t>
+  </si>
+  <si>
+    <t>20-PIN SWD</t>
+  </si>
+  <si>
+    <t>MICRO SD</t>
+  </si>
+  <si>
+    <t>101-00660-68-6</t>
+  </si>
+  <si>
+    <t>2908-05WB-MG</t>
+  </si>
+  <si>
+    <t>3M</t>
+  </si>
+  <si>
+    <t>PIN RECEPTACLE</t>
   </si>
 </sst>
 </file>
@@ -401,7 +452,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -430,6 +481,15 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1919,7 +1979,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H54"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -2196,6 +2256,648 @@
         <v>97</v>
       </c>
     </row>
+    <row r="11" ht="26" customHeight="1">
+      <c r="A11" s="5"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+    </row>
+    <row r="12" ht="26" customHeight="1">
+      <c r="A12" t="s" s="2">
+        <v>99</v>
+      </c>
+      <c r="B12" t="s" s="2">
+        <v>100</v>
+      </c>
+      <c r="C12" t="s" s="2">
+        <v>67</v>
+      </c>
+      <c r="D12" t="s" s="2">
+        <v>2</v>
+      </c>
+      <c r="E12" t="s" s="2">
+        <v>2</v>
+      </c>
+      <c r="F12" t="s" s="2">
+        <v>2</v>
+      </c>
+      <c r="G12" t="s" s="2">
+        <v>2</v>
+      </c>
+      <c r="H12" t="s" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" ht="26" customHeight="1">
+      <c r="A13" t="s" s="5">
+        <v>3</v>
+      </c>
+      <c r="B13" t="s" s="6">
+        <v>101</v>
+      </c>
+      <c r="C13" t="s" s="6">
+        <v>102</v>
+      </c>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+    </row>
+    <row r="14" ht="26" customHeight="1">
+      <c r="A14" t="s" s="3">
+        <v>103</v>
+      </c>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+    </row>
+    <row r="15" ht="26" customHeight="1">
+      <c r="A15" t="s" s="5">
+        <v>83</v>
+      </c>
+      <c r="B15" t="s" s="6">
+        <v>84</v>
+      </c>
+      <c r="C15" t="s" s="6">
+        <v>84</v>
+      </c>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+    </row>
+    <row r="16" ht="26" customHeight="1">
+      <c r="A16" t="s" s="3">
+        <v>86</v>
+      </c>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+    </row>
+    <row r="17" ht="26" customHeight="1">
+      <c r="A17" t="s" s="5">
+        <v>88</v>
+      </c>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
+    </row>
+    <row r="18" ht="26" customHeight="1">
+      <c r="A18" t="s" s="3">
+        <v>91</v>
+      </c>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+    </row>
+    <row r="19" ht="26" customHeight="1">
+      <c r="A19" t="s" s="5">
+        <v>19</v>
+      </c>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
+    </row>
+    <row r="20" ht="26" customHeight="1">
+      <c r="A20" t="s" s="3">
+        <v>21</v>
+      </c>
+      <c r="B20" t="s" s="4">
+        <v>95</v>
+      </c>
+      <c r="C20" t="s" s="4">
+        <v>95</v>
+      </c>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+    </row>
+    <row r="21" ht="26" customHeight="1">
+      <c r="A21" t="s" s="5">
+        <v>96</v>
+      </c>
+      <c r="B21" t="s" s="6">
+        <v>97</v>
+      </c>
+      <c r="C21" t="s" s="6">
+        <v>97</v>
+      </c>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+    </row>
+    <row r="22" ht="26" customHeight="1">
+      <c r="A22" s="3"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+    </row>
+    <row r="23" ht="26" customHeight="1">
+      <c r="A23" t="s" s="2">
+        <v>104</v>
+      </c>
+      <c r="B23" t="s" s="2">
+        <v>105</v>
+      </c>
+      <c r="C23" t="s" s="2">
+        <v>2</v>
+      </c>
+      <c r="D23" t="s" s="2">
+        <v>2</v>
+      </c>
+      <c r="E23" t="s" s="2">
+        <v>2</v>
+      </c>
+      <c r="F23" t="s" s="2">
+        <v>2</v>
+      </c>
+      <c r="G23" t="s" s="2">
+        <v>2</v>
+      </c>
+      <c r="H23" t="s" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" ht="26" customHeight="1">
+      <c r="A24" t="s" s="3">
+        <v>3</v>
+      </c>
+      <c r="B24" t="s" s="4">
+        <v>106</v>
+      </c>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
+    </row>
+    <row r="25" ht="26" customHeight="1">
+      <c r="A25" t="s" s="5">
+        <v>107</v>
+      </c>
+      <c r="B25" t="s" s="6">
+        <v>108</v>
+      </c>
+      <c r="C25" t="s" s="6">
+        <v>109</v>
+      </c>
+      <c r="D25" t="s" s="6">
+        <v>110</v>
+      </c>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="10"/>
+    </row>
+    <row r="26" ht="26" customHeight="1">
+      <c r="A26" t="s" s="3">
+        <v>83</v>
+      </c>
+      <c r="B26" t="s" s="4">
+        <v>84</v>
+      </c>
+      <c r="C26" t="s" s="4">
+        <v>85</v>
+      </c>
+      <c r="D26" t="s" s="4">
+        <v>85</v>
+      </c>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
+    </row>
+    <row r="27" ht="26" customHeight="1">
+      <c r="A27" t="s" s="5">
+        <v>86</v>
+      </c>
+      <c r="B27" s="10"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="10"/>
+    </row>
+    <row r="28" ht="26" customHeight="1">
+      <c r="A28" t="s" s="3">
+        <v>88</v>
+      </c>
+      <c r="B28" s="11"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="11"/>
+    </row>
+    <row r="29" ht="26" customHeight="1">
+      <c r="A29" t="s" s="5">
+        <v>91</v>
+      </c>
+      <c r="B29" s="10"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="10"/>
+      <c r="H29" s="10"/>
+    </row>
+    <row r="30" ht="26" customHeight="1">
+      <c r="A30" t="s" s="3">
+        <v>19</v>
+      </c>
+      <c r="B30" s="11"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="11"/>
+    </row>
+    <row r="31" ht="26" customHeight="1">
+      <c r="A31" t="s" s="5">
+        <v>21</v>
+      </c>
+      <c r="B31" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="C31" t="s" s="6">
+        <v>95</v>
+      </c>
+      <c r="D31" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="E31" s="10"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="10"/>
+    </row>
+    <row r="32" ht="26" customHeight="1">
+      <c r="A32" t="s" s="3">
+        <v>96</v>
+      </c>
+      <c r="B32" t="s" s="4">
+        <v>98</v>
+      </c>
+      <c r="C32" t="s" s="4">
+        <v>98</v>
+      </c>
+      <c r="D32" t="s" s="4">
+        <v>98</v>
+      </c>
+      <c r="E32" s="11"/>
+      <c r="F32" s="11"/>
+      <c r="G32" s="11"/>
+      <c r="H32" s="11"/>
+    </row>
+    <row r="33" ht="26" customHeight="1">
+      <c r="A33" s="5"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="10"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="10"/>
+      <c r="H33" s="10"/>
+    </row>
+    <row r="34" ht="26" customHeight="1">
+      <c r="A34" t="s" s="2">
+        <v>111</v>
+      </c>
+      <c r="B34" t="s" s="2">
+        <v>112</v>
+      </c>
+      <c r="C34" t="s" s="2">
+        <v>113</v>
+      </c>
+      <c r="D34" t="s" s="2">
+        <v>2</v>
+      </c>
+      <c r="E34" t="s" s="2">
+        <v>2</v>
+      </c>
+      <c r="F34" t="s" s="2">
+        <v>2</v>
+      </c>
+      <c r="G34" t="s" s="2">
+        <v>2</v>
+      </c>
+      <c r="H34" t="s" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" ht="26" customHeight="1">
+      <c r="A35" t="s" s="5">
+        <v>3</v>
+      </c>
+      <c r="B35" t="s" s="12">
+        <v>76</v>
+      </c>
+      <c r="C35" t="s" s="6">
+        <v>114</v>
+      </c>
+      <c r="D35" s="10"/>
+      <c r="E35" s="10"/>
+      <c r="F35" s="10"/>
+      <c r="G35" s="10"/>
+      <c r="H35" s="10"/>
+    </row>
+    <row r="36" ht="26" customHeight="1">
+      <c r="A36" t="s" s="3">
+        <v>107</v>
+      </c>
+      <c r="B36" s="11"/>
+      <c r="C36" s="11"/>
+      <c r="D36" s="11"/>
+      <c r="E36" s="11"/>
+      <c r="F36" s="11"/>
+      <c r="G36" s="11"/>
+      <c r="H36" s="11"/>
+    </row>
+    <row r="37" ht="26" customHeight="1">
+      <c r="A37" t="s" s="5">
+        <v>83</v>
+      </c>
+      <c r="B37" s="10"/>
+      <c r="C37" s="10"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="10"/>
+      <c r="F37" s="10"/>
+      <c r="G37" s="10"/>
+      <c r="H37" s="10"/>
+    </row>
+    <row r="38" ht="26" customHeight="1">
+      <c r="A38" t="s" s="3">
+        <v>86</v>
+      </c>
+      <c r="B38" s="11"/>
+      <c r="C38" s="11"/>
+      <c r="D38" s="11"/>
+      <c r="E38" s="11"/>
+      <c r="F38" s="11"/>
+      <c r="G38" s="11"/>
+      <c r="H38" s="11"/>
+    </row>
+    <row r="39" ht="26" customHeight="1">
+      <c r="A39" t="s" s="5">
+        <v>88</v>
+      </c>
+      <c r="B39" s="10"/>
+      <c r="C39" s="10"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="10"/>
+      <c r="F39" s="10"/>
+      <c r="G39" s="10"/>
+      <c r="H39" s="10"/>
+    </row>
+    <row r="40" ht="26" customHeight="1">
+      <c r="A40" t="s" s="3">
+        <v>91</v>
+      </c>
+      <c r="B40" s="11"/>
+      <c r="C40" s="11"/>
+      <c r="D40" s="11"/>
+      <c r="E40" s="11"/>
+      <c r="F40" s="11"/>
+      <c r="G40" s="11"/>
+      <c r="H40" s="11"/>
+    </row>
+    <row r="41" ht="26" customHeight="1">
+      <c r="A41" t="s" s="5">
+        <v>19</v>
+      </c>
+      <c r="B41" s="10"/>
+      <c r="C41" s="10"/>
+      <c r="D41" s="10"/>
+      <c r="E41" s="10"/>
+      <c r="F41" s="10"/>
+      <c r="G41" s="10"/>
+      <c r="H41" s="10"/>
+    </row>
+    <row r="42" ht="26" customHeight="1">
+      <c r="A42" t="s" s="3">
+        <v>21</v>
+      </c>
+      <c r="B42" t="s" s="4">
+        <v>22</v>
+      </c>
+      <c r="C42" t="s" s="4">
+        <v>22</v>
+      </c>
+      <c r="D42" s="11"/>
+      <c r="E42" s="11"/>
+      <c r="F42" s="11"/>
+      <c r="G42" s="11"/>
+      <c r="H42" s="11"/>
+    </row>
+    <row r="43" ht="26" customHeight="1">
+      <c r="A43" t="s" s="5">
+        <v>96</v>
+      </c>
+      <c r="B43" t="s" s="6">
+        <v>97</v>
+      </c>
+      <c r="C43" t="s" s="6">
+        <v>97</v>
+      </c>
+      <c r="D43" s="10"/>
+      <c r="E43" s="10"/>
+      <c r="F43" s="10"/>
+      <c r="G43" s="10"/>
+      <c r="H43" s="10"/>
+    </row>
+    <row r="44" ht="26" customHeight="1">
+      <c r="A44" s="3"/>
+      <c r="B44" s="4"/>
+      <c r="C44" s="4"/>
+      <c r="D44" s="11"/>
+      <c r="E44" s="11"/>
+      <c r="F44" s="11"/>
+      <c r="G44" s="11"/>
+      <c r="H44" s="11"/>
+    </row>
+    <row r="45" ht="26" customHeight="1">
+      <c r="A45" t="s" s="2">
+        <v>115</v>
+      </c>
+      <c r="B45" t="s" s="2">
+        <v>2</v>
+      </c>
+      <c r="C45" t="s" s="2">
+        <v>2</v>
+      </c>
+      <c r="D45" t="s" s="2">
+        <v>2</v>
+      </c>
+      <c r="E45" t="s" s="2">
+        <v>2</v>
+      </c>
+      <c r="F45" t="s" s="2">
+        <v>2</v>
+      </c>
+      <c r="G45" t="s" s="2">
+        <v>2</v>
+      </c>
+      <c r="H45" t="s" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" ht="26" customHeight="1">
+      <c r="A46" t="s" s="3">
+        <v>3</v>
+      </c>
+      <c r="B46" s="11"/>
+      <c r="C46" s="11"/>
+      <c r="D46" s="11"/>
+      <c r="E46" s="11"/>
+      <c r="F46" s="11"/>
+      <c r="G46" s="11"/>
+      <c r="H46" s="11"/>
+    </row>
+    <row r="47" ht="26" customHeight="1">
+      <c r="A47" t="s" s="5">
+        <v>107</v>
+      </c>
+      <c r="B47" s="10"/>
+      <c r="C47" s="10"/>
+      <c r="D47" s="10"/>
+      <c r="E47" s="10"/>
+      <c r="F47" s="10"/>
+      <c r="G47" s="10"/>
+      <c r="H47" s="10"/>
+    </row>
+    <row r="48" ht="26" customHeight="1">
+      <c r="A48" t="s" s="3">
+        <v>83</v>
+      </c>
+      <c r="B48" s="11"/>
+      <c r="C48" s="11"/>
+      <c r="D48" s="11"/>
+      <c r="E48" s="11"/>
+      <c r="F48" s="11"/>
+      <c r="G48" s="11"/>
+      <c r="H48" s="11"/>
+    </row>
+    <row r="49" ht="26" customHeight="1">
+      <c r="A49" t="s" s="5">
+        <v>86</v>
+      </c>
+      <c r="B49" s="10"/>
+      <c r="C49" s="10"/>
+      <c r="D49" s="10"/>
+      <c r="E49" s="10"/>
+      <c r="F49" s="10"/>
+      <c r="G49" s="10"/>
+      <c r="H49" s="10"/>
+    </row>
+    <row r="50" ht="26" customHeight="1">
+      <c r="A50" t="s" s="3">
+        <v>88</v>
+      </c>
+      <c r="B50" s="11"/>
+      <c r="C50" s="11"/>
+      <c r="D50" s="11"/>
+      <c r="E50" s="11"/>
+      <c r="F50" s="11"/>
+      <c r="G50" s="11"/>
+      <c r="H50" s="11"/>
+    </row>
+    <row r="51" ht="26" customHeight="1">
+      <c r="A51" t="s" s="5">
+        <v>91</v>
+      </c>
+      <c r="B51" s="10"/>
+      <c r="C51" s="10"/>
+      <c r="D51" s="10"/>
+      <c r="E51" s="10"/>
+      <c r="F51" s="10"/>
+      <c r="G51" s="10"/>
+      <c r="H51" s="10"/>
+    </row>
+    <row r="52" ht="26" customHeight="1">
+      <c r="A52" t="s" s="3">
+        <v>19</v>
+      </c>
+      <c r="B52" s="11"/>
+      <c r="C52" s="11"/>
+      <c r="D52" s="11"/>
+      <c r="E52" s="11"/>
+      <c r="F52" s="11"/>
+      <c r="G52" s="11"/>
+      <c r="H52" s="11"/>
+    </row>
+    <row r="53" ht="26" customHeight="1">
+      <c r="A53" t="s" s="5">
+        <v>21</v>
+      </c>
+      <c r="B53" t="s" s="6">
+        <v>95</v>
+      </c>
+      <c r="C53" t="s" s="6">
+        <v>95</v>
+      </c>
+      <c r="D53" t="s" s="6">
+        <v>95</v>
+      </c>
+      <c r="E53" s="10"/>
+      <c r="F53" s="10"/>
+      <c r="G53" s="10"/>
+      <c r="H53" s="10"/>
+    </row>
+    <row r="54" ht="26" customHeight="1">
+      <c r="A54" t="s" s="3">
+        <v>96</v>
+      </c>
+      <c r="B54" t="s" s="4">
+        <v>98</v>
+      </c>
+      <c r="C54" t="s" s="4">
+        <v>98</v>
+      </c>
+      <c r="D54" t="s" s="4">
+        <v>98</v>
+      </c>
+      <c r="E54" s="11"/>
+      <c r="F54" s="11"/>
+      <c r="G54" s="11"/>
+      <c r="H54" s="11"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>